<commit_message>
Audio interface refactor & costs
</commit_message>
<xml_diff>
--- a/costs.xlsx
+++ b/costs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Turret\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C343B4C7-8314-42A7-ACED-A9BE0C25CD8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075F1D6E-6F83-487E-8224-B52667A1F613}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{631432DC-88FD-44C9-835E-AA5AF69119B2}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>wzmacniacz audio</t>
   </si>
@@ -62,15 +62,9 @@
     <t>Mazur</t>
   </si>
   <si>
-    <t>Ja</t>
-  </si>
-  <si>
     <t>adapter USB-microUSB</t>
   </si>
   <si>
-    <t>razem zł:</t>
-  </si>
-  <si>
     <t>laser</t>
   </si>
   <si>
@@ -84,14 +78,41 @@
   </si>
   <si>
     <t>wzmacniacz audio raz jeszcze</t>
+  </si>
+  <si>
+    <t>silnik krokowy x 2</t>
+  </si>
+  <si>
+    <t>wzmacniacz audio po raz trzeci</t>
+  </si>
+  <si>
+    <t>siłownik x 2</t>
+  </si>
+  <si>
+    <t>łącznie zł:</t>
+  </si>
+  <si>
+    <t>suma razem:</t>
+  </si>
+  <si>
+    <t>Salata</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -120,8 +141,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -436,175 +458,202 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6783E2E-B51C-4E9E-BE6D-F3DA4BCDCF59}">
-  <dimension ref="D3:K16"/>
+  <dimension ref="B2:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="39.28515625" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
+    <col min="10" max="10" width="21.28515625" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="F3" t="s">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>3.84</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2">
+        <f>SUM(G5:G1000000)</f>
+        <v>132.738</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2">
+        <f>SUM(L5:L1000000)</f>
+        <v>193.5976</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <f>G2+L2</f>
+        <v>326.3356</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1.96</v>
+      </c>
+      <c r="G5">
+        <f>F5*$C$2</f>
+        <v>7.5263999999999998</v>
+      </c>
+      <c r="J5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5">
+        <v>24.9</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>1.26</v>
+      </c>
+      <c r="G6">
+        <f>F6*$C$2</f>
+        <v>4.8384</v>
+      </c>
+      <c r="J6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6">
+        <v>19.989999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>9.98</v>
+      </c>
+      <c r="G7">
+        <f>F7*$C$2</f>
+        <v>38.3232</v>
+      </c>
+      <c r="J7" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>57.75</v>
+      </c>
+      <c r="J8" t="s">
         <v>11</v>
       </c>
-      <c r="G3">
-        <f>SUM(G6:G39)</f>
-        <v>210.59800000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="F5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="L8">
+        <v>23.98</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9">
+        <v>16.3</v>
+      </c>
+      <c r="J9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9">
+        <v>17.28</v>
+      </c>
+      <c r="L9">
+        <f>K9*$C$2</f>
+        <v>66.355199999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10">
         <v>3</v>
       </c>
-      <c r="K5">
-        <v>3.84</v>
-      </c>
-    </row>
-    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>1.96</v>
-      </c>
-      <c r="G6">
-        <f>F6*$K$5</f>
-        <v>7.5263999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7">
-        <v>1.26</v>
-      </c>
-      <c r="G7">
-        <f>F7*$K$5</f>
-        <v>4.8384</v>
-      </c>
-    </row>
-    <row r="8" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="J10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K10">
+        <v>2.81</v>
+      </c>
+      <c r="L10">
+        <f>K10*$C$2</f>
+        <v>10.7904</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11">
         <v>5</v>
       </c>
-      <c r="F8">
-        <v>9.98</v>
-      </c>
-      <c r="G8">
-        <f>F8*$K$5</f>
-        <v>38.3232</v>
-      </c>
-    </row>
-    <row r="9" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9">
-        <v>57.75</v>
-      </c>
-    </row>
-    <row r="10" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10">
-        <v>24.9</v>
-      </c>
-    </row>
-    <row r="11" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11">
-        <v>19.989999999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12">
-        <v>8.99</v>
-      </c>
-    </row>
-    <row r="13" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13">
-        <v>23.98</v>
-      </c>
-    </row>
-    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14">
-        <v>16.3</v>
-      </c>
-    </row>
-    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16">
-        <v>5</v>
+      <c r="J11" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11">
+        <v>10.050000000000001</v>
+      </c>
+      <c r="L11">
+        <f>K11*$C$2</f>
+        <v>38.591999999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
The costs are piling up
</commit_message>
<xml_diff>
--- a/costs.xlsx
+++ b/costs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Turret\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C97A081-6BE3-4402-9457-BCC85A7E4D57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D818C1C-4A38-4C3A-BFDD-5155B82FEE21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{631432DC-88FD-44C9-835E-AA5AF69119B2}"/>
   </bookViews>
@@ -80,9 +80,6 @@
     <t>wzmacniacz audio raz jeszcze</t>
   </si>
   <si>
-    <t>silnik krokowy x 2</t>
-  </si>
-  <si>
     <t>wzmacniacz audio po raz trzeci</t>
   </si>
   <si>
@@ -114,6 +111,9 @@
   </si>
   <si>
     <t>profil kątownik aluminiowy 45x45x3 20mm</t>
+  </si>
+  <si>
+    <t>silnik krokowy nema17 x 2</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
   <dimension ref="B2:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,14 +503,14 @@
         <v>3.84</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G2">
         <f>SUM(G5:G1000000)</f>
         <v>279.81799999999998</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L2">
         <f>SUM(L5:L1000000)</f>
@@ -519,7 +519,7 @@
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <f>G2+L2</f>
@@ -539,7 +539,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>1</v>
@@ -624,7 +624,7 @@
         <v>16.3</v>
       </c>
       <c r="J9" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="K9">
         <v>17.28</v>
@@ -642,7 +642,7 @@
         <v>3</v>
       </c>
       <c r="J10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K10">
         <v>2.81</v>
@@ -660,7 +660,7 @@
         <v>5</v>
       </c>
       <c r="J11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K11">
         <v>10.050000000000001</v>
@@ -672,13 +672,13 @@
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G12">
         <v>60</v>
       </c>
       <c r="J12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L12">
         <v>9.16</v>
@@ -686,13 +686,13 @@
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G13">
         <v>50</v>
       </c>
       <c r="J13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L13">
         <v>13.96</v>
@@ -700,13 +700,13 @@
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G14">
         <v>37.08</v>
       </c>
       <c r="J14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L14">
         <v>15.39</v>

</xml_diff>

<commit_message>
First version of Arduino side board program
</commit_message>
<xml_diff>
--- a/costs.xlsx
+++ b/costs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projekt Turret\Turret\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Turret\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92735D26-FDC0-4729-98CF-41B8B955D771}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E90E78-6A53-4417-8756-0CAC0219571D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{631432DC-88FD-44C9-835E-AA5AF69119B2}"/>
   </bookViews>
@@ -20,17 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t>wzmacniacz audio</t>
   </si>
@@ -147,6 +142,9 @@
   </si>
   <si>
     <t>przewody połączeniowe x 10</t>
+  </si>
+  <si>
+    <t>strata zł</t>
   </si>
 </sst>
 </file>
@@ -509,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6783E2E-B51C-4E9E-BE6D-F3DA4BCDCF59}">
-  <dimension ref="B2:L26"/>
+  <dimension ref="B2:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,7 +759,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="17" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J17" t="s">
         <v>29</v>
       </c>
@@ -769,7 +767,7 @@
         <v>2.66</v>
       </c>
     </row>
-    <row r="18" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J18" t="s">
         <v>30</v>
       </c>
@@ -778,7 +776,7 @@
         <v>10.08</v>
       </c>
     </row>
-    <row r="19" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J19" t="s">
         <v>31</v>
       </c>
@@ -786,7 +784,7 @@
         <v>11.46</v>
       </c>
     </row>
-    <row r="20" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J20" t="s">
         <v>32</v>
       </c>
@@ -794,7 +792,7 @@
         <v>12.26</v>
       </c>
     </row>
-    <row r="21" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J21" t="s">
         <v>33</v>
       </c>
@@ -802,7 +800,7 @@
         <v>9.89</v>
       </c>
     </row>
-    <row r="22" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J22" t="s">
         <v>34</v>
       </c>
@@ -810,7 +808,7 @@
         <v>5.42</v>
       </c>
     </row>
-    <row r="23" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J23" t="s">
         <v>35</v>
       </c>
@@ -819,7 +817,7 @@
         <v>55.16</v>
       </c>
     </row>
-    <row r="24" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J24" t="s">
         <v>36</v>
       </c>
@@ -827,7 +825,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J25" t="s">
         <v>37</v>
       </c>
@@ -835,12 +833,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="10:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J26" t="s">
         <v>38</v>
       </c>
       <c r="L26">
         <v>4.5</v>
+      </c>
+    </row>
+    <row r="30" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>39</v>
+      </c>
+      <c r="F30">
+        <f>G5+G6+G11+L10+L19</f>
+        <v>39.615200000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
initial protocol setup for ESP
</commit_message>
<xml_diff>
--- a/costs.xlsx
+++ b/costs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>kurs dolara:</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>sterownik do silników krokowych drv8825 x 3</t>
+  </si>
+  <si>
+    <t>potencjometr do lutofnicy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">goldpin socket+header </t>
   </si>
 </sst>
 </file>
@@ -478,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,7 +513,7 @@
       </c>
       <c r="G2">
         <f>SUM(G5:G1000000)</f>
-        <v>336.78800000000001</v>
+        <v>346.78800000000001</v>
       </c>
       <c r="K2" t="s">
         <v>1</v>
@@ -523,7 +529,7 @@
       </c>
       <c r="C3">
         <f>G2+L2</f>
-        <v>711.99559999999997</v>
+        <v>721.99559999999997</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
@@ -741,6 +747,12 @@
       </c>
     </row>
     <row r="17" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
       <c r="J17" t="s">
         <v>29</v>
       </c>
@@ -749,6 +761,12 @@
       </c>
     </row>
     <row r="18" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18">
+        <v>8</v>
+      </c>
       <c r="J18" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Succesful connection between RsPI and ESP device. First implementation of stepper motor movement in gimbal achieved.
</commit_message>
<xml_diff>
--- a/costs.xlsx
+++ b/costs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="50">
   <si>
     <t>kurs dolara:</t>
   </si>
@@ -101,9 +101,6 @@
     <t>4x łożysko liniowe 6x12x19</t>
   </si>
   <si>
-    <t>3x łożysko liniowe 6x12x32</t>
-  </si>
-  <si>
     <t>profil kątownik aluminiowy 45x45x3 20mm</t>
   </si>
   <si>
@@ -156,6 +153,27 @@
   </si>
   <si>
     <t xml:space="preserve">goldpin socket+header </t>
+  </si>
+  <si>
+    <t>3x łożysko liniowe 6x12x32 (LM06LUU)</t>
+  </si>
+  <si>
+    <t>3x sensor hala as5600</t>
+  </si>
+  <si>
+    <t>paczka przewodów</t>
+  </si>
+  <si>
+    <t>ładowarka somostel 65W</t>
+  </si>
+  <si>
+    <t>Lutownica usbC</t>
+  </si>
+  <si>
+    <t>2x łożysko kulkowe 6807 2RS</t>
+  </si>
+  <si>
+    <t>przewody v2 10m 26 AWG 4 cores</t>
   </si>
 </sst>
 </file>
@@ -199,9 +217,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,20 +505,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
     <col min="5" max="5" width="40.85546875" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="9" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" style="3" customWidth="1"/>
     <col min="9" max="9" width="10.140625" customWidth="1"/>
     <col min="10" max="10" width="44.42578125" customWidth="1"/>
     <col min="11" max="11" width="10.140625" customWidth="1"/>
+    <col min="12" max="12" width="8.5703125" style="3"/>
     <col min="14" max="14" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -505,22 +527,22 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>3.84</v>
+      <c r="C2" s="2">
+        <v>4.0199999999999996</v>
       </c>
       <c r="F2" t="s">
         <v>1</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="3">
         <f>SUM(G5:G1000000)</f>
-        <v>346.78800000000001</v>
+        <v>560.36680000000001</v>
       </c>
       <c r="K2" t="s">
         <v>1</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="3">
         <f>SUM(L5:L1000000)</f>
-        <v>375.20759999999996</v>
+        <v>436.82279999999997</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
@@ -529,7 +551,7 @@
       </c>
       <c r="C3">
         <f>G2+L2</f>
-        <v>721.99559999999997</v>
+        <v>997.18959999999993</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
@@ -539,7 +561,7 @@
       <c r="F4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H4" s="1"/>
@@ -550,7 +572,7 @@
       <c r="K4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -561,14 +583,14 @@
       <c r="F5">
         <v>1.96</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="3">
         <f>F5*$C$2</f>
-        <v>7.5263999999999998</v>
+        <v>7.8791999999999991</v>
       </c>
       <c r="J5" t="s">
         <v>8</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="3">
         <v>24.9</v>
       </c>
     </row>
@@ -579,14 +601,14 @@
       <c r="F6">
         <v>1.26</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="3">
         <f>F6*$C$2</f>
-        <v>4.8384</v>
+        <v>5.0651999999999999</v>
       </c>
       <c r="J6" t="s">
         <v>10</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="3">
         <v>19.989999999999998</v>
       </c>
     </row>
@@ -597,14 +619,14 @@
       <c r="F7">
         <v>9.98</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="3">
         <f>F7*$C$2</f>
-        <v>38.3232</v>
+        <v>40.119599999999998</v>
       </c>
       <c r="J7" t="s">
         <v>12</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="3">
         <v>8.99</v>
       </c>
     </row>
@@ -612,13 +634,13 @@
       <c r="E8" t="s">
         <v>13</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="3">
         <v>57.75</v>
       </c>
       <c r="J8" t="s">
         <v>14</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="3">
         <v>23.98</v>
       </c>
     </row>
@@ -626,7 +648,7 @@
       <c r="E9" t="s">
         <v>15</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="3">
         <v>16.3</v>
       </c>
       <c r="J9" t="s">
@@ -635,16 +657,16 @@
       <c r="K9">
         <v>17.28</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="3">
         <f>K9*$C$2</f>
-        <v>66.355199999999996</v>
+        <v>69.465599999999995</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>17</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="3">
         <v>3</v>
       </c>
       <c r="J10" t="s">
@@ -653,16 +675,16 @@
       <c r="K10">
         <v>2.81</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="3">
         <f>K10*$C$2</f>
-        <v>10.7904</v>
+        <v>11.296199999999999</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
         <v>19</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="3">
         <v>5</v>
       </c>
       <c r="J11" t="s">
@@ -671,22 +693,22 @@
       <c r="K11">
         <v>10.050000000000001</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="3">
         <f>K11*$C$2</f>
-        <v>38.591999999999999</v>
+        <v>40.400999999999996</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
         <v>21</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="3">
         <v>60</v>
       </c>
       <c r="J12" t="s">
         <v>22</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="3">
         <v>9.16</v>
       </c>
     </row>
@@ -694,163 +716,207 @@
       <c r="E13" t="s">
         <v>23</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="3">
         <v>50</v>
       </c>
       <c r="J13" t="s">
         <v>24</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="3">
         <v>13.96</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="3">
+        <v>37.08</v>
+      </c>
+      <c r="J14" t="s">
         <v>25</v>
       </c>
-      <c r="G14">
-        <v>37.08</v>
-      </c>
-      <c r="J14" t="s">
-        <v>26</v>
-      </c>
-      <c r="L14">
+      <c r="L14" s="3">
         <v>15.39</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15">
+        <v>39</v>
+      </c>
+      <c r="G15" s="3">
         <v>23.38</v>
       </c>
       <c r="J15" t="s">
-        <v>27</v>
-      </c>
-      <c r="L15">
+        <v>26</v>
+      </c>
+      <c r="L15" s="3">
         <v>7.07</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16">
+        <v>40</v>
+      </c>
+      <c r="G16" s="3">
         <v>33.590000000000003</v>
       </c>
       <c r="J16" t="s">
-        <v>28</v>
-      </c>
-      <c r="L16">
+        <v>27</v>
+      </c>
+      <c r="L16" s="3">
         <v>2.6</v>
       </c>
     </row>
     <row r="17" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17">
+        <v>41</v>
+      </c>
+      <c r="G17" s="3">
         <v>2</v>
       </c>
       <c r="J17" t="s">
-        <v>29</v>
-      </c>
-      <c r="L17">
+        <v>28</v>
+      </c>
+      <c r="L17" s="3">
         <v>2.66</v>
       </c>
     </row>
     <row r="18" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>43</v>
-      </c>
-      <c r="G18">
+        <v>42</v>
+      </c>
+      <c r="G18" s="3">
         <v>8</v>
       </c>
       <c r="J18" t="s">
-        <v>30</v>
-      </c>
-      <c r="L18">
+        <v>29</v>
+      </c>
+      <c r="L18" s="3">
         <f>4*2.52</f>
         <v>10.08</v>
       </c>
     </row>
     <row r="19" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>44</v>
+      </c>
+      <c r="G19" s="3">
+        <v>20.66</v>
+      </c>
       <c r="J19" t="s">
+        <v>30</v>
+      </c>
+      <c r="L19" s="3">
+        <v>11.46</v>
+      </c>
+    </row>
+    <row r="20" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="3">
+        <v>20.350000000000001</v>
+      </c>
+      <c r="J20" t="s">
         <v>31</v>
       </c>
-      <c r="L19">
-        <v>11.46</v>
-      </c>
-    </row>
-    <row r="20" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="J20" t="s">
+      <c r="L20" s="3">
+        <v>12.26</v>
+      </c>
+    </row>
+    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G21" s="3">
+        <v>43</v>
+      </c>
+      <c r="J21" t="s">
         <v>32</v>
       </c>
-      <c r="L20">
-        <v>12.26</v>
-      </c>
-    </row>
-    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="J21" t="s">
+      <c r="L21" s="3">
+        <v>9.89</v>
+      </c>
+    </row>
+    <row r="22" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22">
+        <v>31.64</v>
+      </c>
+      <c r="G22" s="3">
+        <f>F22*C2</f>
+        <v>127.19279999999999</v>
+      </c>
+      <c r="J22" t="s">
         <v>33</v>
       </c>
-      <c r="L21">
-        <v>9.89</v>
-      </c>
-    </row>
-    <row r="22" spans="5:12" x14ac:dyDescent="0.25">
-      <c r="J22" t="s">
-        <v>34</v>
-      </c>
-      <c r="L22">
+      <c r="L22" s="3">
         <v>5.42</v>
       </c>
     </row>
     <row r="23" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J23" t="s">
-        <v>35</v>
-      </c>
-      <c r="L23">
+        <v>34</v>
+      </c>
+      <c r="L23" s="3">
         <f>2*27.58</f>
         <v>55.16</v>
       </c>
     </row>
     <row r="24" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J24" t="s">
-        <v>36</v>
-      </c>
-      <c r="L24">
+        <v>35</v>
+      </c>
+      <c r="L24" s="3">
         <v>9</v>
       </c>
     </row>
     <row r="25" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J25" t="s">
-        <v>37</v>
-      </c>
-      <c r="L25">
+        <v>36</v>
+      </c>
+      <c r="L25" s="3">
         <v>13</v>
       </c>
     </row>
     <row r="26" spans="5:12" x14ac:dyDescent="0.25">
       <c r="J26" t="s">
-        <v>38</v>
-      </c>
-      <c r="L26">
+        <v>37</v>
+      </c>
+      <c r="L26" s="3">
         <v>4.5</v>
+      </c>
+    </row>
+    <row r="27" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>49</v>
+      </c>
+      <c r="L27" s="3">
+        <v>35.200000000000003</v>
+      </c>
+    </row>
+    <row r="28" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="J28" t="s">
+        <v>48</v>
+      </c>
+      <c r="L28" s="3">
+        <v>20.99</v>
       </c>
     </row>
     <row r="30" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F30">
         <f>G5+G6+G11+L10+L19+G16</f>
-        <v>73.205200000000005</v>
+        <v>74.290599999999998</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>